<commit_message>
worked all mechanics, ui do later
</commit_message>
<xml_diff>
--- a/combo.xlsx
+++ b/combo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="25185" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="25185" windowHeight="12600" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="stats" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="188">
   <si>
     <t>spades</t>
   </si>
@@ -341,15 +341,6 @@
     <t>\\Наделяет способностью вампиризм за каждую обычную атаку, а за каст вампиризм удвоенные рейты</t>
   </si>
   <si>
-    <t>\\увеличенный блокрейт</t>
-  </si>
-  <si>
-    <t>\\повышенная бронебойность</t>
-  </si>
-  <si>
-    <t>\\обладает врожденной регенерацией от недостающего % здоровья каждый ход.</t>
-  </si>
-  <si>
     <t xml:space="preserve">\\универсальный </t>
   </si>
   <si>
@@ -509,9 +500,6 @@
     <t>уменьшение выносливости = AGI%k1+(k2+kn)%(k3+kn)</t>
   </si>
   <si>
-    <t>Уменьшение крит урона = AGI%k1+(k2+kn)%(k3+kn)</t>
-  </si>
-  <si>
     <t>уменьшение урона = AGI%k1+(k2+kn)%(k3+kn)</t>
   </si>
   <si>
@@ -554,9 +542,6 @@
     <t>восстановление выносливости = END%k1+(k2+kn)%(k3+kn)</t>
   </si>
   <si>
-    <t>восстановление крит урона = END%k1+(k2+kn)%(k3+kn)</t>
-  </si>
-  <si>
     <t>восстановление силы лечения = END%k1+(k2+kn)%(k3+kn)</t>
   </si>
   <si>
@@ -596,9 +581,6 @@
     <t>увеличение выносливости = INT%k1+(k2+kn)%(k3+kn)</t>
   </si>
   <si>
-    <t>увеличение крит урона = INT%k1+(k2+kn)%(k3+kn)</t>
-  </si>
-  <si>
     <t>увеличение силы лечения = INT%k1+(k2+kn)%(k3+kn)</t>
   </si>
   <si>
@@ -662,9 +644,6 @@
     <t>пробивание брони</t>
   </si>
   <si>
-    <t>вампиризм</t>
-  </si>
-  <si>
     <t>Сила восстановления жизней</t>
   </si>
   <si>
@@ -672,6 +651,21 @@
   </si>
   <si>
     <t xml:space="preserve">\\ пришлось внести дополнительные статы, так как комбо могут изменять их множитель, для взаимодейсвтия. Что бы не писать в какие то переменные,  решил так бороться </t>
+  </si>
+  <si>
+    <t>вампиризм ( life leech)</t>
+  </si>
+  <si>
+    <t>\\ защита это порог, который урон должен пройти, что бы нанести хоть какой то урон</t>
+  </si>
+  <si>
+    <t>\\обладает врожденной регенерацией от недостающего % здоровья каждый ход. = currHP = currHP + (baseHP%currHP)/10</t>
+  </si>
+  <si>
+    <t>\\повышенная бронебойность = enemyDEF - enemyDEF%10</t>
+  </si>
+  <si>
+    <t>\\увеличенный блокрейт, если использует щит + 5% к блокированию атаки.</t>
   </si>
 </sst>
 </file>
@@ -1199,10 +1193,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D18"/>
+  <dimension ref="B1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,14 +1206,14 @@
     <col min="4" max="4" width="51.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="10" t="s">
         <v>31</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="24" t="s">
         <v>21</v>
       </c>
@@ -1228,7 +1222,7 @@
       </c>
       <c r="D2" s="11"/>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="24" t="s">
         <v>22</v>
       </c>
@@ -1237,7 +1231,7 @@
       </c>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="24" t="s">
         <v>23</v>
       </c>
@@ -1246,7 +1240,7 @@
       </c>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
         <v>24</v>
       </c>
@@ -1255,14 +1249,14 @@
       </c>
       <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="11"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
         <v>25</v>
       </c>
@@ -1270,10 +1264,10 @@
         <v>37</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
         <v>26</v>
       </c>
@@ -1283,8 +1277,11 @@
       <c r="D8" s="19" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="26" t="s">
         <v>27</v>
       </c>
@@ -1295,7 +1292,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
         <v>28</v>
       </c>
@@ -1306,7 +1303,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="28" t="s">
         <v>29</v>
       </c>
@@ -1317,7 +1314,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="28" t="s">
         <v>30</v>
       </c>
@@ -1328,45 +1325,45 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="39" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C13" s="40" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D13" s="39"/>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="D14" s="39"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="39" t="s">
+        <v>177</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>180</v>
+      </c>
+      <c r="D15" s="39"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="C16" s="40" t="s">
         <v>181</v>
-      </c>
-      <c r="C14" s="40" t="s">
-        <v>186</v>
-      </c>
-      <c r="D14" s="39"/>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="39" t="s">
-        <v>183</v>
-      </c>
-      <c r="C15" s="40" t="s">
-        <v>187</v>
-      </c>
-      <c r="D15" s="39"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="39" t="s">
-        <v>184</v>
-      </c>
-      <c r="C16" s="40" t="s">
-        <v>188</v>
       </c>
       <c r="D16" s="39"/>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="38" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -1380,7 +1377,7 @@
   <dimension ref="A1:X26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,7 +1405,7 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -1446,13 +1443,13 @@
         <v>74</v>
       </c>
       <c r="L2" s="19" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="M2" s="19" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N2" s="19" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="O2" s="17" t="s">
         <v>29</v>
@@ -1973,7 +1970,7 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
@@ -1996,7 +1993,7 @@
         <v>67</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H14" s="23" t="s">
         <v>68</v>
@@ -2008,7 +2005,7 @@
         <v>66</v>
       </c>
       <c r="K14" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
@@ -2096,7 +2093,7 @@
         <v>16.5</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
@@ -2153,7 +2150,7 @@
         <v>23</v>
       </c>
       <c r="K17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -2197,7 +2194,7 @@
         <v>34.5</v>
       </c>
       <c r="K18" t="s">
-        <v>79</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -2241,7 +2238,7 @@
         <v>38.5</v>
       </c>
       <c r="K19" t="s">
-        <v>80</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -2285,7 +2282,7 @@
         <v>39.5</v>
       </c>
       <c r="K20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -2329,7 +2326,7 @@
         <v>45</v>
       </c>
       <c r="K21" t="s">
-        <v>81</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -2373,7 +2370,7 @@
         <v>17</v>
       </c>
       <c r="K22" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -2417,12 +2414,12 @@
         <v>22.5</v>
       </c>
       <c r="K23" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2432,10 +2429,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2458,142 +2455,161 @@
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:14" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
     </row>
     <row r="5" spans="1:14" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
+      <c r="A5" s="4"/>
     </row>
     <row r="6" spans="1:14" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-    </row>
-    <row r="7" spans="1:14" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B7" s="32" t="s">
+      <c r="A6" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:14" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="G7" s="34"/>
+    </row>
+    <row r="8" spans="1:14" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>136</v>
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>110</v>
       </c>
       <c r="D8" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+    </row>
+    <row r="11" spans="1:14" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E11" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="1:14" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="E12" s="30" t="s">
         <v>156</v>
-      </c>
-      <c r="G8" s="34"/>
-    </row>
-    <row r="9" spans="1:14" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>145</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-    </row>
-    <row r="12" spans="1:14" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="30" t="s">
-        <v>176</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>146</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>160</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -2605,19 +2621,19 @@
     </row>
     <row r="13" spans="1:14" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>132</v>
+        <v>103</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>130</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -2627,21 +2643,21 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="30" t="s">
-        <v>106</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>133</v>
+        <v>11</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>131</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -2651,22 +2667,16 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:14" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="E15" s="30" t="s">
-        <v>163</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
@@ -2677,19 +2687,19 @@
     </row>
     <row r="16" spans="1:14" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -2699,131 +2709,107 @@
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="1:14" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" s="30" t="s">
+        <v>167</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="30" t="s">
         <v>174</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="D17" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="E17" s="30" t="s">
-        <v>165</v>
-      </c>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-    </row>
-    <row r="18" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="30" t="s">
-        <v>173</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="D18" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="E18" s="30" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="30" t="s">
-        <v>172</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="D19" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="30" t="s">
-        <v>177</v>
-      </c>
-      <c r="C20" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="E20" s="30" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>178</v>
-      </c>
-      <c r="C21" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="D21" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="30" t="s">
-        <v>179</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="30" t="s">
-        <v>180</v>
-      </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="35" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C23" t="s">
         <v>59</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D23" t="s">
         <v>61</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E23" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2869,16 +2855,16 @@
         <v>0</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2886,16 +2872,16 @@
         <v>1</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>103</v>
-      </c>
       <c r="E8" s="11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2903,16 +2889,16 @@
         <v>2</v>
       </c>
       <c r="B9" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>118</v>
-      </c>
       <c r="D9" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>119</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2920,21 +2906,21 @@
         <v>3</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C10" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="E10" s="11" t="s">
         <v>120</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -2942,7 +2928,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -2950,7 +2936,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
@@ -2958,7 +2944,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>

</xml_diff>

<commit_message>
little changes,bot can only attack, some bugs available
</commit_message>
<xml_diff>
--- a/combo.xlsx
+++ b/combo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="25185" windowHeight="12600" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="25185" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="stats" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="190">
   <si>
     <t>spades</t>
   </si>
@@ -666,6 +666,12 @@
   </si>
   <si>
     <t>\\увеличенный блокрейт, если использует щит + 5% к блокированию атаки.</t>
+  </si>
+  <si>
+    <t>формула для пробивания брони простая = def - def(из комбо) - атака</t>
+  </si>
+  <si>
+    <t>формулы для урона = def - атака</t>
   </si>
 </sst>
 </file>
@@ -1193,10 +1199,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E18"/>
+  <dimension ref="B1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1366,6 +1372,16 @@
         <v>182</v>
       </c>
     </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="38" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>188</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1376,8 +1392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,7 +1415,7 @@
     <col min="15" max="15" width="6.140625" customWidth="1"/>
     <col min="17" max="17" width="5.7109375" customWidth="1"/>
     <col min="18" max="18" width="5.85546875" customWidth="1"/>
-    <col min="19" max="19" width="6" customWidth="1"/>
+    <col min="19" max="19" width="4.28515625" customWidth="1"/>
     <col min="20" max="20" width="6.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1463,6 +1479,9 @@
       <c r="R2" s="17" t="s">
         <v>76</v>
       </c>
+      <c r="S2" s="36" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -1519,6 +1538,9 @@
       <c r="R3" s="18">
         <v>1.75</v>
       </c>
+      <c r="S3" s="36">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -1575,6 +1597,9 @@
       <c r="R4" s="18">
         <v>2.5</v>
       </c>
+      <c r="S4" s="36">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -1631,6 +1656,9 @@
       <c r="R5" s="18">
         <v>2</v>
       </c>
+      <c r="S5" s="36">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
@@ -1687,6 +1715,9 @@
       <c r="R6" s="18">
         <v>0.75</v>
       </c>
+      <c r="S6" s="36">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
@@ -1743,6 +1774,9 @@
       <c r="R7" s="18">
         <v>0.5</v>
       </c>
+      <c r="S7" s="36">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
@@ -1799,6 +1833,9 @@
       <c r="R8" s="18">
         <v>0.5</v>
       </c>
+      <c r="S8" s="36">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
@@ -1855,6 +1892,9 @@
       <c r="R9" s="18">
         <v>0.5</v>
       </c>
+      <c r="S9" s="36">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
@@ -1911,6 +1951,9 @@
       <c r="R10" s="18">
         <v>2.25</v>
       </c>
+      <c r="S10" s="36">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
@@ -1967,6 +2010,9 @@
       <c r="R11" s="18">
         <v>2</v>
       </c>
+      <c r="S11" s="36">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -2045,8 +2091,8 @@
         <v>130.80000000000001</v>
       </c>
       <c r="J15" s="37">
-        <f>B15/2</f>
-        <v>18</v>
+        <f>S3+B15/2</f>
+        <v>23</v>
       </c>
       <c r="K15" t="s">
         <v>78</v>
@@ -2089,8 +2135,8 @@
         <v>183.4</v>
       </c>
       <c r="J16" s="37">
-        <f t="shared" ref="J16:J23" si="0">B16/2</f>
-        <v>16.5</v>
+        <f t="shared" ref="J16:J23" si="0">S4+B16/2</f>
+        <v>20.5</v>
       </c>
       <c r="K16" s="9" t="s">
         <v>81</v>
@@ -2147,7 +2193,7 @@
       </c>
       <c r="J17" s="37">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="K17" t="s">
         <v>86</v>
@@ -2191,7 +2237,7 @@
       </c>
       <c r="J18" s="37">
         <f t="shared" si="0"/>
-        <v>34.5</v>
+        <v>40.5</v>
       </c>
       <c r="K18" t="s">
         <v>187</v>
@@ -2235,7 +2281,7 @@
       </c>
       <c r="J19" s="37">
         <f t="shared" si="0"/>
-        <v>38.5</v>
+        <v>44.5</v>
       </c>
       <c r="K19" t="s">
         <v>186</v>
@@ -2279,7 +2325,7 @@
       </c>
       <c r="J20" s="37">
         <f t="shared" si="0"/>
-        <v>39.5</v>
+        <v>45.5</v>
       </c>
       <c r="K20" t="s">
         <v>87</v>
@@ -2323,7 +2369,7 @@
       </c>
       <c r="J21" s="37">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="K21" t="s">
         <v>185</v>
@@ -2367,7 +2413,7 @@
       </c>
       <c r="J22" s="37">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="K22" t="s">
         <v>109</v>
@@ -2411,7 +2457,7 @@
       </c>
       <c r="J23" s="37">
         <f t="shared" si="0"/>
-        <v>22.5</v>
+        <v>27.5</v>
       </c>
       <c r="K23" t="s">
         <v>79</v>
@@ -2431,8 +2477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>